<commit_message>
fix : bar plots show all files
</commit_message>
<xml_diff>
--- a/Affy/ARI/ARI_normed_binary_results.xlsx
+++ b/Affy/ARI/ARI_normed_binary_results.xlsx
@@ -487,31 +487,31 @@
         <v>11</v>
       </c>
       <c r="B2">
-        <v>0.7304281394824405</v>
+        <v>0.5089441903256321</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>0.4943333713621592</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0.3941101905926027</v>
+        <v>0.3246404326649622</v>
       </c>
       <c r="F2">
-        <v>0.1762291725437023</v>
+        <v>0.3586383285908433</v>
       </c>
       <c r="G2">
-        <v>0.1762291725437023</v>
+        <v>0.3586383285908433</v>
       </c>
       <c r="H2">
-        <v>0.2325718259086036</v>
+        <v>0.1794793107198907</v>
       </c>
       <c r="I2">
-        <v>0.2920997974838273</v>
+        <v>0.2610012569162791</v>
       </c>
       <c r="J2">
-        <v>0.2920997974838273</v>
+        <v>0.5942751998756042</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -519,7 +519,7 @@
         <v>12</v>
       </c>
       <c r="B3">
-        <v>0.4324503388473908</v>
+        <v>0.3923116926485909</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -528,22 +528,22 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0.4566174203134199</v>
+        <v>0.4908480066013919</v>
       </c>
       <c r="F3">
-        <v>0.6010157066109535</v>
+        <v>0.554957660978823</v>
       </c>
       <c r="G3">
-        <v>0.6010157066109535</v>
+        <v>0.554957660978823</v>
       </c>
       <c r="H3">
-        <v>0.3359392870395315</v>
+        <v>0.6500194412739141</v>
       </c>
       <c r="I3">
-        <v>0.6147775222296673</v>
+        <v>0.6102808058241208</v>
       </c>
       <c r="J3">
-        <v>0.5176674395689751</v>
+        <v>0.4686367749667203</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -551,31 +551,31 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <v>0.1997571259994113</v>
+        <v>0.224450920129413</v>
       </c>
       <c r="C4">
-        <v>0.1196893884944973</v>
+        <v>0.5179264704491768</v>
       </c>
       <c r="D4">
-        <v>0.387724766157155</v>
+        <v>0.05103467618520385</v>
       </c>
       <c r="E4">
-        <v>0.3253399433890664</v>
+        <v>0.2655360114382984</v>
       </c>
       <c r="F4">
-        <v>0.05248151996559756</v>
+        <v>0.1887897996101501</v>
       </c>
       <c r="G4">
-        <v>0.05248151996559756</v>
+        <v>0.1887897996101501</v>
       </c>
       <c r="H4">
-        <v>0.1434251091429048</v>
+        <v>0.2136556847703774</v>
       </c>
       <c r="I4">
-        <v>0.1154603645598353</v>
+        <v>0.1893997023084638</v>
       </c>
       <c r="J4">
-        <v>0.3054205118740995</v>
+        <v>0.09180260090716087</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -583,10 +583,10 @@
         <v>14</v>
       </c>
       <c r="B5">
-        <v>0.8490787306869069</v>
+        <v>0.7780876219875478</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>-0.02472840254945134</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -615,31 +615,31 @@
         <v>15</v>
       </c>
       <c r="B6">
-        <v>0.2343459392436454</v>
+        <v>0.2220561864913329</v>
       </c>
       <c r="C6">
-        <v>0.01278563656147994</v>
+        <v>0.1612076331529478</v>
       </c>
       <c r="D6">
-        <v>-0.01812849906691543</v>
+        <v>0.1952695269526953</v>
       </c>
       <c r="E6">
-        <v>0.3131090851933354</v>
+        <v>0.1442483262325015</v>
       </c>
       <c r="F6">
-        <v>0.1893491124260355</v>
+        <v>0.2865013774104683</v>
       </c>
       <c r="G6">
-        <v>0.1893491124260355</v>
+        <v>0.2865013774104683</v>
       </c>
       <c r="H6">
-        <v>0.2223451327433629</v>
+        <v>0.2102960478343299</v>
       </c>
       <c r="I6">
-        <v>0.3549198365293932</v>
+        <v>0.3163329161451815</v>
       </c>
       <c r="J6">
-        <v>0.1228981962702538</v>
+        <v>0.2907662082514735</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -647,31 +647,31 @@
         <v>16</v>
       </c>
       <c r="B7">
-        <v>0.2036599763872492</v>
+        <v>0.08588162782127758</v>
       </c>
       <c r="C7">
-        <v>-0.03687054548842415</v>
+        <v>0.07482671326787527</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>0.02355523043160223</v>
       </c>
       <c r="E7">
-        <v>0.2907092907092907</v>
+        <v>0.2511841651758604</v>
       </c>
       <c r="F7">
-        <v>0.06364678899082575</v>
+        <v>0.03270642201834869</v>
       </c>
       <c r="G7">
-        <v>0.06364678899082575</v>
+        <v>0.03270642201834869</v>
       </c>
       <c r="H7">
-        <v>0.05866031217724366</v>
+        <v>-0.02103211009174305</v>
       </c>
       <c r="I7">
-        <v>0.2919838245435679</v>
+        <v>-0.02615503290715429</v>
       </c>
       <c r="J7">
-        <v>0.01898356723819393</v>
+        <v>0.2619408900464274</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -679,31 +679,31 @@
         <v>17</v>
       </c>
       <c r="B8">
-        <v>0.1047603773189638</v>
+        <v>0.1726881347951491</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>0.1923971217807718</v>
       </c>
       <c r="D8">
-        <v>0.4155105009135648</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>0.2448285366307571</v>
+        <v>0.2965919384057971</v>
       </c>
       <c r="F8">
-        <v>0.02289465744330147</v>
+        <v>-0.05504256060165497</v>
       </c>
       <c r="G8">
-        <v>0.02289465744330147</v>
+        <v>-0.05504256060165497</v>
       </c>
       <c r="H8">
-        <v>0.287244927508253</v>
+        <v>0.4315771524583482</v>
       </c>
       <c r="I8">
-        <v>0.2406045982806607</v>
+        <v>0.4495362037934376</v>
       </c>
       <c r="J8">
-        <v>0.081168125587714</v>
+        <v>0.2145429743060812</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -711,7 +711,7 @@
         <v>18</v>
       </c>
       <c r="B9">
-        <v>-0.01711364610013112</v>
+        <v>0.01517832801143781</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -720,22 +720,22 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0.8947811391584896</v>
+        <v>0.8228271770322414</v>
       </c>
       <c r="F9">
-        <v>-0.1101844581472504</v>
+        <v>0.6003473083602083</v>
       </c>
       <c r="G9">
-        <v>-0.1101844581472504</v>
+        <v>0.6003473083602083</v>
       </c>
       <c r="H9">
-        <v>0.4004174157209667</v>
+        <v>0.1305616848814452</v>
       </c>
       <c r="I9">
-        <v>0.3135952881114071</v>
+        <v>0.9200414896919314</v>
       </c>
       <c r="J9">
-        <v>0.636586467933918</v>
+        <v>0.06494837344412167</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -743,16 +743,16 @@
         <v>19</v>
       </c>
       <c r="B10">
-        <v>0.222427647016995</v>
+        <v>0.04248245289988915</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>-0.03971119133574001</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>0.3128995863106431</v>
+        <v>0.09954158480681068</v>
       </c>
       <c r="F10">
         <v>-0.05762933857236419</v>
@@ -761,13 +761,13 @@
         <v>-0.05762933857236419</v>
       </c>
       <c r="H10">
-        <v>0.004238810259357777</v>
+        <v>0.06033940917661845</v>
       </c>
       <c r="I10">
-        <v>0.2329007365836548</v>
+        <v>-0.00678179402922467</v>
       </c>
       <c r="J10">
-        <v>0.3128995863106431</v>
+        <v>0.140262599260948</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -775,31 +775,31 @@
         <v>20</v>
       </c>
       <c r="B11">
-        <v>0.07834428109686166</v>
+        <v>0.08434343434343435</v>
       </c>
       <c r="C11">
-        <v>0.0284273694630042</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>-0.004700507972343765</v>
       </c>
       <c r="E11">
-        <v>0.1508037350038413</v>
+        <v>0.1019917402896127</v>
       </c>
       <c r="F11">
-        <v>0.027698252640783</v>
+        <v>0.04508496450849644</v>
       </c>
       <c r="G11">
-        <v>0.027698252640783</v>
+        <v>0.04508496450849644</v>
       </c>
       <c r="H11">
-        <v>0.09363397016134478</v>
+        <v>0.04427525712697285</v>
       </c>
       <c r="I11">
-        <v>0.08059733761620903</v>
+        <v>0.1069334692837114</v>
       </c>
       <c r="J11">
-        <v>0.05503166205213961</v>
+        <v>0.09799751395704749</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -807,31 +807,31 @@
         <v>21</v>
       </c>
       <c r="B12">
-        <v>0.1363636363636364</v>
+        <v>-0.03583473861720073</v>
       </c>
       <c r="C12">
-        <v>-0.01027960526315787</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>-0.01027960526315787</v>
+        <v>-0.005319148936170364</v>
       </c>
       <c r="E12">
-        <v>0.007518796992481256</v>
+        <v>0.002099958000840043</v>
       </c>
       <c r="F12">
-        <v>-0.01027960526315787</v>
+        <v>-0.03409090909090909</v>
       </c>
       <c r="G12">
-        <v>-0.01027960526315787</v>
+        <v>-0.03409090909090909</v>
       </c>
       <c r="H12">
-        <v>-0.03714647530603622</v>
+        <v>0.01451679800912478</v>
       </c>
       <c r="I12">
-        <v>0.002099958000840043</v>
+        <v>-0.001686340640809492</v>
       </c>
       <c r="J12">
-        <v>-0.03846153846153842</v>
+        <v>-0.02574926129168418</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -839,31 +839,31 @@
         <v>22</v>
       </c>
       <c r="B13">
+        <v>-0.08450704225352125</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0.05688622754491006</v>
+      </c>
+      <c r="F13">
+        <v>-0.024390243902439</v>
+      </c>
+      <c r="G13">
+        <v>-0.024390243902439</v>
+      </c>
+      <c r="H13">
         <v>-0.0405405405405406</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>-0.05538461538461534</v>
-      </c>
-      <c r="E13">
-        <v>-0.02997275204359669</v>
-      </c>
-      <c r="F13">
-        <v>-0.02162162162162168</v>
-      </c>
-      <c r="G13">
-        <v>-0.02162162162162168</v>
-      </c>
-      <c r="H13">
-        <v>0.0576923076923077</v>
-      </c>
       <c r="I13">
-        <v>0.06539509536784745</v>
+        <v>0.1812865497076024</v>
       </c>
       <c r="J13">
-        <v>-0.01111111111111107</v>
+        <v>0.01355013550135503</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -871,31 +871,31 @@
         <v>23</v>
       </c>
       <c r="B14">
+        <v>0.04281767955801098</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
         <v>0.03076923076923077</v>
       </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
       <c r="E14">
-        <v>0.04106628242074932</v>
+        <v>-0.003429355281207231</v>
       </c>
       <c r="F14">
-        <v>-0.02888583218707011</v>
+        <v>0.1970802919708028</v>
       </c>
       <c r="G14">
-        <v>-0.02888583218707011</v>
+        <v>0.1970802919708028</v>
       </c>
       <c r="H14">
-        <v>-0.06552706552706561</v>
+        <v>-0.01167883211678843</v>
       </c>
       <c r="I14">
-        <v>0.01650618982118298</v>
+        <v>0.04281767955801098</v>
       </c>
       <c r="J14">
-        <v>0.04106628242074932</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -903,31 +903,31 @@
         <v>24</v>
       </c>
       <c r="B15">
-        <v>0.2838591678097851</v>
+        <v>0.3743869209809265</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>0.0143742255266419</v>
       </c>
       <c r="D15">
-        <v>0.108234075608493</v>
+        <v>0.165769000598444</v>
       </c>
       <c r="E15">
-        <v>0.2934326967862133</v>
+        <v>0.2144776766363242</v>
       </c>
       <c r="F15">
-        <v>0.3929824561403509</v>
+        <v>0.3024827024827025</v>
       </c>
       <c r="G15">
-        <v>0.3929824561403509</v>
+        <v>0.3024827024827025</v>
       </c>
       <c r="H15">
-        <v>0.1956403269754768</v>
+        <v>0.5777987718469533</v>
       </c>
       <c r="I15">
-        <v>0.4161690399632522</v>
+        <v>0.1857914416285833</v>
       </c>
       <c r="J15">
-        <v>0.3598513011152416</v>
+        <v>0.1987676056338028</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -935,31 +935,31 @@
         <v>25</v>
       </c>
       <c r="B16">
-        <v>0.3040669042602412</v>
+        <v>0.3624811388968273</v>
       </c>
       <c r="C16">
-        <v>0.154184047465066</v>
+        <v>0.03490904536133276</v>
       </c>
       <c r="D16">
-        <v>0.003241200620253871</v>
+        <v>-0.001629632488204126</v>
       </c>
       <c r="E16">
-        <v>0.4024384970474587</v>
+        <v>0.4929564166194816</v>
       </c>
       <c r="F16">
-        <v>0.08743621917892597</v>
+        <v>0.2456420626559125</v>
       </c>
       <c r="G16">
-        <v>0.08743621917892597</v>
+        <v>0.2456420626559125</v>
       </c>
       <c r="H16">
-        <v>0.3559332485354896</v>
+        <v>0.3528218428011595</v>
       </c>
       <c r="I16">
-        <v>0.3382656733646953</v>
+        <v>0.3426105006068903</v>
       </c>
       <c r="J16">
-        <v>0.366506486815039</v>
+        <v>0.2234327044307217</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -967,31 +967,31 @@
         <v>26</v>
       </c>
       <c r="B17">
-        <v>0.02135988426516884</v>
+        <v>0.1467170656586868</v>
       </c>
       <c r="C17">
-        <v>0.0243284338570706</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>0.1025292357900461</v>
       </c>
       <c r="E17">
-        <v>-0.02807775377969762</v>
+        <v>0.01357658039881208</v>
       </c>
       <c r="F17">
-        <v>-0.0196212835232628</v>
+        <v>-0.03959683225341973</v>
       </c>
       <c r="G17">
-        <v>-0.0196212835232628</v>
+        <v>-0.03959683225341973</v>
       </c>
       <c r="H17">
-        <v>0.1832838353839627</v>
+        <v>0.1421051149959182</v>
       </c>
       <c r="I17">
-        <v>0.189883006480936</v>
+        <v>-0.006508991947928046</v>
       </c>
       <c r="J17">
-        <v>0.1081171829094266</v>
+        <v>0.1447084233261339</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -999,31 +999,31 @@
         <v>27</v>
       </c>
       <c r="B18">
-        <v>0.04403503036315536</v>
+        <v>0.03518437202263319</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>0.03138581299500854</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>0.005357593271323863</v>
       </c>
       <c r="E18">
-        <v>0.03747248805472274</v>
+        <v>0.0293527236723549</v>
       </c>
       <c r="F18">
-        <v>-0.001413021872838721</v>
+        <v>0.03489933096170147</v>
       </c>
       <c r="G18">
-        <v>-0.001413021872838721</v>
+        <v>0.03489933096170147</v>
       </c>
       <c r="H18">
-        <v>0.03702265724227415</v>
+        <v>0.0298199743222094</v>
       </c>
       <c r="I18">
-        <v>0.03518437202263319</v>
+        <v>0.06446305198588806</v>
       </c>
       <c r="J18">
-        <v>0.05476258236826547</v>
+        <v>0.06483324433984185</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1031,31 +1031,31 @@
         <v>28</v>
       </c>
       <c r="B19">
-        <v>0.4555578732869413</v>
+        <v>0.4246698766347226</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>-0.001682722548086535</v>
       </c>
       <c r="D19">
-        <v>0.003785140195593154</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>0.5052616400087594</v>
+        <v>0.4314287805532591</v>
       </c>
       <c r="F19">
-        <v>0.2899266732300576</v>
+        <v>0.3036008406515629</v>
       </c>
       <c r="G19">
-        <v>0.2899266732300576</v>
+        <v>0.3036008406515629</v>
       </c>
       <c r="H19">
-        <v>0.4757302675323959</v>
+        <v>0.3907868125394266</v>
       </c>
       <c r="I19">
-        <v>0.3355549417306919</v>
+        <v>0.446825073863188</v>
       </c>
       <c r="J19">
-        <v>0.5093685520899153</v>
+        <v>0.4493924241640341</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1063,7 +1063,7 @@
         <v>29</v>
       </c>
       <c r="B20">
-        <v>0.193657856038611</v>
+        <v>-0.02035278154681141</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1072,22 +1072,22 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>0.06521492999207465</v>
+        <v>0.4327097163548582</v>
       </c>
       <c r="F20">
-        <v>0.006792452830188683</v>
+        <v>0.3268505955073119</v>
       </c>
       <c r="G20">
-        <v>0.006792452830188683</v>
+        <v>0.3268505955073119</v>
       </c>
       <c r="H20">
-        <v>0.04211956521739121</v>
+        <v>-0.01992678416424493</v>
       </c>
       <c r="I20">
-        <v>0.1222410865874364</v>
+        <v>0.04226415094339623</v>
       </c>
       <c r="J20">
-        <v>0.06521492999207465</v>
+        <v>-0.01403138201569091</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1095,7 +1095,7 @@
         <v>30</v>
       </c>
       <c r="B21">
-        <v>0.04634476504204373</v>
+        <v>-0.05106795963914094</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -1104,22 +1104,22 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>-0.06824740644500887</v>
+        <v>-0.01851905628050766</v>
       </c>
       <c r="F21">
-        <v>-0.001038839445391085</v>
+        <v>0.1062404390290867</v>
       </c>
       <c r="G21">
-        <v>-0.001038839445391085</v>
+        <v>0.1062404390290867</v>
       </c>
       <c r="H21">
-        <v>-0.02353019869256723</v>
+        <v>0.0005100182149363802</v>
       </c>
       <c r="I21">
-        <v>-0.02379908494024687</v>
+        <v>-0.002308123641547955</v>
       </c>
       <c r="J21">
-        <v>-0.01420171588132246</v>
+        <v>0.1394124820813454</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1127,31 +1127,31 @@
         <v>31</v>
       </c>
       <c r="B22">
-        <v>-0.01907179122267334</v>
+        <v>-0.0145470234833475</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>-0.005530368669925899</v>
       </c>
       <c r="D22">
-        <v>-0.006364484183606912</v>
+        <v>-0.007376670918393435</v>
       </c>
       <c r="E22">
-        <v>0.015023821612953</v>
+        <v>0.002157865200333181</v>
       </c>
       <c r="F22">
-        <v>-0.007135853039285706</v>
+        <v>0.001800914066815311</v>
       </c>
       <c r="G22">
-        <v>-0.007135853039285706</v>
+        <v>0.001800914066815311</v>
       </c>
       <c r="H22">
-        <v>-0.0004122269707654638</v>
+        <v>-0.007235863445365188</v>
       </c>
       <c r="I22">
-        <v>0.0001893596956370147</v>
+        <v>-0.007917137795485647</v>
       </c>
       <c r="J22">
-        <v>0.01233802358647477</v>
+        <v>0.02098811055254978</v>
       </c>
     </row>
   </sheetData>

</xml_diff>